<commit_message>
Frankrig og tyskland skulle lige bytte index i frac excel
</commit_message>
<xml_diff>
--- a/Project 1/FracOver20.xlsx
+++ b/Project 1/FracOver20.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0d9fef8507f605b/Dokumenter/Skole/Kandidat/3. semester/AIO/Projects/Advanced-IO/Project 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0d9fef8507f605b/Dokumenter/Skole/Kandidat/3. semester/AIO/Advanced-IO/Project 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{66DB436E-DDBF-44E4-AFBB-16653A2E033C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7227AE83-4213-41A5-B15C-8A3676B05E34}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{66DB436E-DDBF-44E4-AFBB-16653A2E033C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E034429-9574-4E5E-AB1D-047D06A92C69}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="3720" windowHeight="4872" xr2:uid="{C3C3B38F-95E8-4AF5-9BE1-5FAB7609B10E}"/>
+    <workbookView xWindow="9204" yWindow="1128" windowWidth="13824" windowHeight="11376" xr2:uid="{C3C3B38F-95E8-4AF5-9BE1-5FAB7609B10E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,7 +404,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF392D96-A338-4FAB-9A49-FED1177E571E}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -437,11 +435,11 @@
         <v>0.68891230926546299</v>
       </c>
       <c r="C2">
+        <f>C3/AVERAGE(B3/B2,D3/D2,E3/E2,F3/F2)</f>
+        <v>0.65664626075716004</v>
+      </c>
+      <c r="D2">
         <v>0.70214354402662815</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D22" si="0">D3/AVERAGE(B3/B2,C3/C2,E3/E2,F3/F2)</f>
-        <v>0.65664626075716004</v>
       </c>
       <c r="E2">
         <v>0.6816651858143663</v>
@@ -458,11 +456,11 @@
         <v>0.68910999794424255</v>
       </c>
       <c r="C3">
+        <f>C4/AVERAGE(B4/B3,D4/D3,E4/E3,F4/F3)</f>
+        <v>0.65734995722700429</v>
+      </c>
+      <c r="D3">
         <v>0.70288157124346018</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>0.65734995722700429</v>
       </c>
       <c r="E3">
         <v>0.6835710473253469</v>
@@ -479,11 +477,11 @@
         <v>0.68978211166371106</v>
       </c>
       <c r="C4">
+        <f>C5/AVERAGE(B5/B4,D5/D4,E5/E4,F5/F4)</f>
+        <v>0.65794421946822224</v>
+      </c>
+      <c r="D4">
         <v>0.70375041484083989</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0.65794421946822224</v>
       </c>
       <c r="E4">
         <v>0.68451160160520175</v>
@@ -500,11 +498,11 @@
         <v>0.69162349578743376</v>
       </c>
       <c r="C5">
+        <f>C6/AVERAGE(B6/B5,D6/D5,E6/E5,F6/F5)</f>
+        <v>0.65878778566293972</v>
+      </c>
+      <c r="D5">
         <v>0.70561221490118053</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0.65878778566293972</v>
       </c>
       <c r="E5">
         <v>0.6842433035693426</v>
@@ -521,11 +519,11 @@
         <v>0.6935553302947034</v>
       </c>
       <c r="C6">
+        <f>C7/AVERAGE(B7/B6,D7/D6,E7/E6,F7/F6)</f>
+        <v>0.65999396944172006</v>
+      </c>
+      <c r="D6">
         <v>0.70824295222172118</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>0.65999396944172006</v>
       </c>
       <c r="E6">
         <v>0.68390400646656491</v>
@@ -542,11 +540,11 @@
         <v>0.69669342256142264</v>
       </c>
       <c r="C7">
+        <f>C8/AVERAGE(B8/B7,D8/D7,E8/E7,F8/F7)</f>
+        <v>0.66163645881984445</v>
+      </c>
+      <c r="D7">
         <v>0.71054473215873637</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>0.66163645881984445</v>
       </c>
       <c r="E7">
         <v>0.68412278898919565</v>
@@ -563,11 +561,11 @@
         <v>0.70026205647278261</v>
       </c>
       <c r="C8">
+        <f>C9/AVERAGE(B9/B8,D9/D8,E9/E8,F9/F8)</f>
+        <v>0.66373302379639953</v>
+      </c>
+      <c r="D8">
         <v>0.71349083092793297</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>0.66373302379639953</v>
       </c>
       <c r="E8">
         <v>0.68477510446947332</v>
@@ -584,11 +582,11 @@
         <v>0.70391982247924378</v>
       </c>
       <c r="C9">
+        <f>C10/AVERAGE(B10/B9,D10/D9,E10/E9,F10/F9)</f>
+        <v>0.6663609281926165</v>
+      </c>
+      <c r="D9">
         <v>0.71712569363794754</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0.6663609281926165</v>
       </c>
       <c r="E9">
         <v>0.6860338357170277</v>
@@ -605,11 +603,11 @@
         <v>0.70785459551205188</v>
       </c>
       <c r="C10">
+        <f>C11/AVERAGE(B11/B10,D11/D10,E11/E10,F11/F10)</f>
+        <v>0.6695490318979852</v>
+      </c>
+      <c r="D10">
         <v>0.72163317224029666</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>0.6695490318979852</v>
       </c>
       <c r="E10">
         <v>0.68805704141155233</v>
@@ -626,11 +624,11 @@
         <v>0.71208335509458065</v>
       </c>
       <c r="C11">
+        <f>C12/AVERAGE(B12/B11,D12/D11,E12/E11,F12/F11)</f>
+        <v>0.67288903720739079</v>
+      </c>
+      <c r="D11">
         <v>0.72613151407847498</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>0.67288903720739079</v>
       </c>
       <c r="E11">
         <v>0.6905910405879836</v>
@@ -647,11 +645,11 @@
         <v>0.71627409536778375</v>
       </c>
       <c r="C12">
+        <f>C13/AVERAGE(B13/B12,D13/D12,E13/E12,F13/F12)</f>
+        <v>0.6765640853399203</v>
+      </c>
+      <c r="D12">
         <v>0.73110097638096294</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0.6765640853399203</v>
       </c>
       <c r="E12">
         <v>0.69415034773060036</v>
@@ -668,11 +666,11 @@
         <v>0.72001051567141228</v>
       </c>
       <c r="C13">
+        <f>C14/AVERAGE(B14/B13,D14/D13,E14/E13,F14/F13)</f>
+        <v>0.68038016752514174</v>
+      </c>
+      <c r="D13">
         <v>0.73598949572635819</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0.68038016752514174</v>
       </c>
       <c r="E13">
         <v>0.69843325743234885</v>
@@ -689,11 +687,11 @@
         <v>0.72264880859059666</v>
       </c>
       <c r="C14">
+        <f>C15/AVERAGE(B15/B14,D15/D14,E15/E14,F15/F14)</f>
+        <v>0.6844960364302165</v>
+      </c>
+      <c r="D14">
         <v>0.74181564183664084</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>0.6844960364302165</v>
       </c>
       <c r="E14">
         <v>0.70373607601887933</v>
@@ -710,11 +708,11 @@
         <v>0.72715070383830738</v>
       </c>
       <c r="C15">
+        <f>C16/AVERAGE(B16/B15,D16/D15,E16/E15,F16/F15)</f>
+        <v>0.68926755883768764</v>
+      </c>
+      <c r="D15">
         <v>0.74840326603305063</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0.68926755883768764</v>
       </c>
       <c r="E15">
         <v>0.70878075823058351</v>
@@ -731,11 +729,11 @@
         <v>0.73112708658043324</v>
       </c>
       <c r="C16">
+        <f>C17/AVERAGE(B17/B16,D17/D16,E17/E16,F17/F16)</f>
+        <v>0.69455170115037446</v>
+      </c>
+      <c r="D16">
         <v>0.75625273328746667</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>0.69455170115037446</v>
       </c>
       <c r="E16">
         <v>0.71449206053971392</v>
@@ -752,11 +750,11 @@
         <v>0.73682629078262618</v>
       </c>
       <c r="C17">
+        <f>C18/AVERAGE(B18/B17,D18/D17,E18/E17,F18/F17)</f>
+        <v>0.7007056842728373</v>
+      </c>
+      <c r="D17">
         <v>0.76468781208406533</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>0.7007056842728373</v>
       </c>
       <c r="E17">
         <v>0.72151307410280197</v>
@@ -773,11 +771,11 @@
         <v>0.74121105864298187</v>
       </c>
       <c r="C18">
+        <f>C19/AVERAGE(B19/B18,D19/D18,E19/E18,F19/F18)</f>
+        <v>0.7060384884926294</v>
+      </c>
+      <c r="D18">
         <v>0.77207530377427092</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>0.7060384884926294</v>
       </c>
       <c r="E18">
         <v>0.72826248104984526</v>
@@ -794,11 +792,11 @@
         <v>0.74475453055023899</v>
       </c>
       <c r="C19">
+        <f>C20/AVERAGE(B20/B19,D20/D19,E20/E19,F20/F19)</f>
+        <v>0.71093005620905891</v>
+      </c>
+      <c r="D19">
         <v>0.77859547051828737</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>0.71093005620905891</v>
       </c>
       <c r="E19">
         <v>0.73532962671788149</v>
@@ -815,11 +813,11 @@
         <v>0.74689500994155766</v>
       </c>
       <c r="C20">
+        <f>C21/AVERAGE(B21/B20,D21/D20,E21/E20,F21/F20)</f>
+        <v>0.71532556923418755</v>
+      </c>
+      <c r="D20">
         <v>0.78531263203079904</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>0.71532556923418755</v>
       </c>
       <c r="E20">
         <v>0.74199964228539883</v>
@@ -836,11 +834,11 @@
         <v>0.74938011276024885</v>
       </c>
       <c r="C21">
+        <f>C22/AVERAGE(B22/B21,D22/D21,E22/E21,F22/F21)</f>
+        <v>0.71898815691657969</v>
+      </c>
+      <c r="D21">
         <v>0.78933863239278723</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>0.71898815691657969</v>
       </c>
       <c r="E21">
         <v>0.74823185943964154</v>
@@ -857,11 +855,11 @@
         <v>0.75159256606145974</v>
       </c>
       <c r="C22">
+        <f>C23/AVERAGE(B23/B22,D23/D22,E23/E22,F23/F22)</f>
+        <v>0.72214454471678635</v>
+      </c>
+      <c r="D22">
         <v>0.79146188195143719</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>0.72214454471678635</v>
       </c>
       <c r="E22">
         <v>0.75485729091923781</v>
@@ -878,10 +876,10 @@
         <v>0.75367996815852645</v>
       </c>
       <c r="C23">
+        <v>0.72261509049397687</v>
+      </c>
+      <c r="D23">
         <v>0.78304447793692411</v>
-      </c>
-      <c r="D23">
-        <v>0.72261509049397687</v>
       </c>
       <c r="E23">
         <v>0.76092481055173311</v>
@@ -898,10 +896,10 @@
         <v>0.75541022412998127</v>
       </c>
       <c r="C24">
+        <v>0.7262035697352085</v>
+      </c>
+      <c r="D24">
         <v>0.78456631667286292</v>
-      </c>
-      <c r="D24">
-        <v>0.7262035697352085</v>
       </c>
       <c r="E24">
         <v>0.77187267599380083</v>
@@ -918,10 +916,10 @@
         <v>0.75692009758530698</v>
       </c>
       <c r="C25">
+        <v>0.72989798632539193</v>
+      </c>
+      <c r="D25">
         <v>0.78508292572419469</v>
-      </c>
-      <c r="D25">
-        <v>0.72989798632539193</v>
       </c>
       <c r="E25">
         <v>0.7770759179004334</v>
@@ -938,10 +936,10 @@
         <v>0.75817124692506832</v>
       </c>
       <c r="C26">
+        <v>0.73340963909237089</v>
+      </c>
+      <c r="D26">
         <v>0.78475094074310303</v>
-      </c>
-      <c r="D26">
-        <v>0.73340963909237089</v>
       </c>
       <c r="E26">
         <v>0.78239392177584643</v>
@@ -958,10 +956,10 @@
         <v>0.75917188897687338</v>
       </c>
       <c r="C27">
+        <v>0.73593257532448841</v>
+      </c>
+      <c r="D27">
         <v>0.78474422722204351</v>
-      </c>
-      <c r="D27">
-        <v>0.73593257532448841</v>
       </c>
       <c r="E27">
         <v>0.78778032132905662</v>
@@ -978,10 +976,10 @@
         <v>0.75988270585751994</v>
       </c>
       <c r="C28">
+        <v>0.73726049248401826</v>
+      </c>
+      <c r="D28">
         <v>0.78453681406223374</v>
-      </c>
-      <c r="D28">
-        <v>0.73726049248401826</v>
       </c>
       <c r="E28">
         <v>0.7924910435448671</v>
@@ -998,10 +996,10 @@
         <v>0.76061436589511389</v>
       </c>
       <c r="C29">
+        <v>0.73816160582694557</v>
+      </c>
+      <c r="D29">
         <v>0.78449528010248037</v>
-      </c>
-      <c r="D29">
-        <v>0.73816160582694557</v>
       </c>
       <c r="E29">
         <v>0.79604793302187882</v>
@@ -1018,10 +1016,10 @@
         <v>0.76151461539850218</v>
       </c>
       <c r="C30">
+        <v>0.73950524372417237</v>
+      </c>
+      <c r="D30">
         <v>0.7847674735016823</v>
-      </c>
-      <c r="D30">
-        <v>0.73950524372417237</v>
       </c>
       <c r="E30">
         <v>0.79884908330165594</v>
@@ -1038,10 +1036,10 @@
         <v>0.76251459796556642</v>
       </c>
       <c r="C31">
+        <v>0.74056770965475505</v>
+      </c>
+      <c r="D31">
         <v>0.78566235183775768</v>
-      </c>
-      <c r="D31">
-        <v>0.74056770965475505</v>
       </c>
       <c r="E31">
         <v>0.80126337947058701</v>

</xml_diff>